<commit_message>
combining AFRICOS data and labs
</commit_message>
<xml_diff>
--- a/data/Sedia® HIV-1 LAg-Avidity EIA ODs results 2.xlsx
+++ b/data/Sedia® HIV-1 LAg-Avidity EIA ODs results 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dokiror\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sempajb\Documents\GitHub\EDCTP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2155B60-7D02-4BAF-B3F2-35DA9CEE8A23}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644B57C2-B00F-4130-930D-AE9A623C2C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EDITTED SHIPPING MANIFEST-IDI E" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2611" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="161">
   <si>
     <t>Date Collected</t>
   </si>
@@ -502,19 +502,7 @@
     <t>ODs</t>
   </si>
   <si>
-    <t>PLATE 1</t>
-  </si>
-  <si>
-    <t>PLATE 2</t>
-  </si>
-  <si>
-    <t>PLATE 3</t>
-  </si>
-  <si>
-    <t>PLATE 4</t>
-  </si>
-  <si>
-    <t>PLATE 5 29/8/2023</t>
+    <t>Plates</t>
   </si>
 </sst>
 </file>
@@ -664,7 +652,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -852,19 +840,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -886,8 +862,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1054,6 +1036,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1099,40 +1090,34 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1488,10 +1473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O120"/>
+  <dimension ref="A1:P120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3:O30"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="S46" sqref="S46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1509,7 +1494,7 @@
     <col min="15" max="15" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1543,14 +1528,16 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="10"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1562,18 +1549,18 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="15">
-        <v>1</v>
-      </c>
-      <c r="M2" s="15">
+      <c r="L2" s="9">
+        <v>1</v>
+      </c>
+      <c r="M2" s="9">
         <v>2</v>
       </c>
-      <c r="N2" s="15">
+      <c r="N2" s="9">
         <v>3</v>
       </c>
-      <c r="O2" s="11"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O2" s="12"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>42053</v>
       </c>
@@ -1616,11 +1603,12 @@
       <c r="N3" s="3">
         <v>3.169</v>
       </c>
-      <c r="O3" s="12" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O3" s="13">
+        <v>1</v>
+      </c>
+      <c r="P3" s="13"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>41893</v>
       </c>
@@ -1663,9 +1651,12 @@
       <c r="N4" s="3">
         <v>3.4529999999999998</v>
       </c>
-      <c r="O4" s="12"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O4" s="14">
+        <v>1</v>
+      </c>
+      <c r="P4" s="14"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>42044</v>
       </c>
@@ -1708,9 +1699,12 @@
       <c r="N5" s="3">
         <v>3.6349999999999998</v>
       </c>
-      <c r="O5" s="12"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O5" s="14">
+        <v>1</v>
+      </c>
+      <c r="P5" s="14"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>42261</v>
       </c>
@@ -1753,9 +1747,12 @@
       <c r="N6" s="3">
         <v>3.4260000000000002</v>
       </c>
-      <c r="O6" s="12"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O6" s="14">
+        <v>1</v>
+      </c>
+      <c r="P6" s="14"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>42439</v>
       </c>
@@ -1798,9 +1795,12 @@
       <c r="N7" s="3">
         <v>3.44</v>
       </c>
-      <c r="O7" s="12"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O7" s="13">
+        <v>1</v>
+      </c>
+      <c r="P7" s="13"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>42430</v>
       </c>
@@ -1843,9 +1843,12 @@
       <c r="N8" s="3">
         <v>3.6480000000000001</v>
       </c>
-      <c r="O8" s="12"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O8" s="14">
+        <v>1</v>
+      </c>
+      <c r="P8" s="14"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>42436</v>
       </c>
@@ -1888,9 +1891,12 @@
       <c r="N9" s="3">
         <v>3.649</v>
       </c>
-      <c r="O9" s="12"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O9" s="14">
+        <v>1</v>
+      </c>
+      <c r="P9" s="14"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>42331</v>
       </c>
@@ -1933,9 +1939,12 @@
       <c r="N10" s="3">
         <v>1.9690000000000001</v>
       </c>
-      <c r="O10" s="12"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O10" s="14">
+        <v>1</v>
+      </c>
+      <c r="P10" s="14"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>42759</v>
       </c>
@@ -1978,9 +1987,12 @@
       <c r="N11" s="3">
         <v>3.734</v>
       </c>
-      <c r="O11" s="12"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O11" s="13">
+        <v>1</v>
+      </c>
+      <c r="P11" s="13"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>42760</v>
       </c>
@@ -2023,9 +2035,12 @@
       <c r="N12" s="3">
         <v>3.387</v>
       </c>
-      <c r="O12" s="12"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O12" s="14">
+        <v>1</v>
+      </c>
+      <c r="P12" s="14"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>42626</v>
       </c>
@@ -2068,9 +2083,12 @@
       <c r="N13" s="3">
         <v>3.6219999999999999</v>
       </c>
-      <c r="O13" s="12"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O13" s="14">
+        <v>1</v>
+      </c>
+      <c r="P13" s="14"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>42598</v>
       </c>
@@ -2113,9 +2131,12 @@
       <c r="N14" s="3">
         <v>2.8450000000000002</v>
       </c>
-      <c r="O14" s="12"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O14" s="14">
+        <v>1</v>
+      </c>
+      <c r="P14" s="14"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>42830</v>
       </c>
@@ -2158,9 +2179,12 @@
       <c r="N15" s="3">
         <v>3.4740000000000002</v>
       </c>
-      <c r="O15" s="12"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O15" s="13">
+        <v>1</v>
+      </c>
+      <c r="P15" s="13"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>42823</v>
       </c>
@@ -2203,9 +2227,12 @@
       <c r="N16" s="3">
         <v>3.0379999999999998</v>
       </c>
-      <c r="O16" s="12"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O16" s="14">
+        <v>1</v>
+      </c>
+      <c r="P16" s="14"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>42991</v>
       </c>
@@ -2248,9 +2275,12 @@
       <c r="N17" s="3">
         <v>3.5049999999999999</v>
       </c>
-      <c r="O17" s="12"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O17" s="14">
+        <v>1</v>
+      </c>
+      <c r="P17" s="14"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>42992</v>
       </c>
@@ -2293,9 +2323,12 @@
       <c r="N18" s="3">
         <v>3.3889999999999998</v>
       </c>
-      <c r="O18" s="12"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O18" s="14">
+        <v>1</v>
+      </c>
+      <c r="P18" s="14"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>42290</v>
       </c>
@@ -2338,9 +2371,12 @@
       <c r="N19" s="3">
         <v>1.45</v>
       </c>
-      <c r="O19" s="12"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O19" s="13">
+        <v>1</v>
+      </c>
+      <c r="P19" s="13"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>42662</v>
       </c>
@@ -2383,9 +2419,12 @@
       <c r="N20" s="3">
         <v>3.7029999999999998</v>
       </c>
-      <c r="O20" s="12"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O20" s="14">
+        <v>1</v>
+      </c>
+      <c r="P20" s="14"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>42656</v>
       </c>
@@ -2428,9 +2467,12 @@
       <c r="N21" s="3">
         <v>2.399</v>
       </c>
-      <c r="O21" s="12"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O21" s="14">
+        <v>1</v>
+      </c>
+      <c r="P21" s="14"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>42663</v>
       </c>
@@ -2473,9 +2515,12 @@
       <c r="N22" s="3">
         <v>2.3759999999999999</v>
       </c>
-      <c r="O22" s="12"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O22" s="14">
+        <v>1</v>
+      </c>
+      <c r="P22" s="14"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>42621</v>
       </c>
@@ -2518,9 +2563,12 @@
       <c r="N23" s="3">
         <v>3.7890000000000001</v>
       </c>
-      <c r="O23" s="12"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O23" s="13">
+        <v>1</v>
+      </c>
+      <c r="P23" s="13"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>42011</v>
       </c>
@@ -2563,9 +2611,12 @@
       <c r="N24" s="3">
         <v>2.1480000000000001</v>
       </c>
-      <c r="O24" s="12"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O24" s="14">
+        <v>1</v>
+      </c>
+      <c r="P24" s="14"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>41771</v>
       </c>
@@ -2608,9 +2659,12 @@
       <c r="N25" s="3">
         <v>2.2040000000000002</v>
       </c>
-      <c r="O25" s="12"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O25" s="14">
+        <v>1</v>
+      </c>
+      <c r="P25" s="14"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>42626</v>
       </c>
@@ -2653,9 +2707,12 @@
       <c r="N26" s="3">
         <v>3.5750000000000002</v>
       </c>
-      <c r="O26" s="12"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O26" s="14">
+        <v>1</v>
+      </c>
+      <c r="P26" s="14"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>42585</v>
       </c>
@@ -2698,9 +2755,12 @@
       <c r="N27" s="3">
         <v>3.5270000000000001</v>
       </c>
-      <c r="O27" s="12"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O27" s="13">
+        <v>1</v>
+      </c>
+      <c r="P27" s="13"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>42677</v>
       </c>
@@ -2743,9 +2803,12 @@
       <c r="N28" s="3">
         <v>3.528</v>
       </c>
-      <c r="O28" s="12"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O28" s="14">
+        <v>1</v>
+      </c>
+      <c r="P28" s="14"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>42669</v>
       </c>
@@ -2788,9 +2851,12 @@
       <c r="N29" s="3">
         <v>1.583</v>
       </c>
-      <c r="O29" s="12"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O29" s="14">
+        <v>1</v>
+      </c>
+      <c r="P29" s="14"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>42670</v>
       </c>
@@ -2833,9 +2899,12 @@
       <c r="N30" s="3">
         <v>3.5139999999999998</v>
       </c>
-      <c r="O30" s="12"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O30" s="14">
+        <v>1</v>
+      </c>
+      <c r="P30" s="14"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>43026</v>
       </c>
@@ -2878,11 +2947,12 @@
       <c r="N31" s="5">
         <v>1.048</v>
       </c>
-      <c r="O31" s="13" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O31" s="13">
+        <v>2</v>
+      </c>
+      <c r="P31" s="13"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>43025</v>
       </c>
@@ -2925,9 +2995,12 @@
       <c r="N32" s="5">
         <v>3.7639999999999998</v>
       </c>
-      <c r="O32" s="13"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O32" s="13">
+        <v>2</v>
+      </c>
+      <c r="P32" s="13"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>43003</v>
       </c>
@@ -2970,9 +3043,12 @@
       <c r="N33" s="5">
         <v>3.33</v>
       </c>
-      <c r="O33" s="13"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O33" s="13">
+        <v>2</v>
+      </c>
+      <c r="P33" s="13"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>43025</v>
       </c>
@@ -3015,9 +3091,12 @@
       <c r="N34" s="5">
         <v>1.7170000000000001</v>
       </c>
-      <c r="O34" s="13"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O34" s="13">
+        <v>2</v>
+      </c>
+      <c r="P34" s="13"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>42940</v>
       </c>
@@ -3060,9 +3139,12 @@
       <c r="N35" s="5">
         <v>2.9169999999999998</v>
       </c>
-      <c r="O35" s="13"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O35" s="13">
+        <v>2</v>
+      </c>
+      <c r="P35" s="13"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>42948</v>
       </c>
@@ -3105,9 +3187,12 @@
       <c r="N36" s="5">
         <v>3.391</v>
       </c>
-      <c r="O36" s="13"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O36" s="13">
+        <v>2</v>
+      </c>
+      <c r="P36" s="13"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>42107</v>
       </c>
@@ -3150,9 +3235,12 @@
       <c r="N37" s="5">
         <v>1.7370000000000001</v>
       </c>
-      <c r="O37" s="13"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O37" s="13">
+        <v>2</v>
+      </c>
+      <c r="P37" s="13"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>42472</v>
       </c>
@@ -3189,15 +3277,18 @@
       <c r="L38" s="5">
         <v>1.4670000000000001</v>
       </c>
-      <c r="M38" s="5">
-        <v>1574</v>
+      <c r="M38" s="18">
+        <v>1.5740000000000001</v>
       </c>
       <c r="N38" s="5">
         <v>1.502</v>
       </c>
-      <c r="O38" s="13"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O38" s="13">
+        <v>2</v>
+      </c>
+      <c r="P38" s="13"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>42851</v>
       </c>
@@ -3240,9 +3331,12 @@
       <c r="N39" s="5">
         <v>1.1220000000000001</v>
       </c>
-      <c r="O39" s="13"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O39" s="13">
+        <v>2</v>
+      </c>
+      <c r="P39" s="13"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>42852</v>
       </c>
@@ -3285,9 +3379,12 @@
       <c r="N40" s="5">
         <v>3.5230000000000001</v>
       </c>
-      <c r="O40" s="13"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O40" s="13">
+        <v>2</v>
+      </c>
+      <c r="P40" s="13"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>43347</v>
       </c>
@@ -3330,9 +3427,12 @@
       <c r="N41" s="5">
         <v>2.3370000000000002</v>
       </c>
-      <c r="O41" s="13"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O41" s="13">
+        <v>2</v>
+      </c>
+      <c r="P41" s="13"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>42877</v>
       </c>
@@ -3375,9 +3475,12 @@
       <c r="N42" s="5">
         <v>3.52</v>
       </c>
-      <c r="O42" s="13"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O42" s="13">
+        <v>2</v>
+      </c>
+      <c r="P42" s="13"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>42879</v>
       </c>
@@ -3420,9 +3523,12 @@
       <c r="N43" s="5">
         <v>3.4220000000000002</v>
       </c>
-      <c r="O43" s="13"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O43" s="13">
+        <v>2</v>
+      </c>
+      <c r="P43" s="13"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>42887</v>
       </c>
@@ -3465,9 +3571,12 @@
       <c r="N44" s="5">
         <v>3.4020000000000001</v>
       </c>
-      <c r="O44" s="13"/>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O44" s="13">
+        <v>2</v>
+      </c>
+      <c r="P44" s="13"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>42037</v>
       </c>
@@ -3510,9 +3619,12 @@
       <c r="N45" s="5">
         <v>1.8939999999999999</v>
       </c>
-      <c r="O45" s="13"/>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O45" s="13">
+        <v>2</v>
+      </c>
+      <c r="P45" s="13"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>42774</v>
       </c>
@@ -3555,9 +3667,12 @@
       <c r="N46" s="5">
         <v>3.58</v>
       </c>
-      <c r="O46" s="13"/>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O46" s="13">
+        <v>2</v>
+      </c>
+      <c r="P46" s="13"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>42774</v>
       </c>
@@ -3600,9 +3715,12 @@
       <c r="N47" s="5">
         <v>3.468</v>
       </c>
-      <c r="O47" s="13"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O47" s="13">
+        <v>2</v>
+      </c>
+      <c r="P47" s="13"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>42774</v>
       </c>
@@ -3645,9 +3763,12 @@
       <c r="N48" s="5">
         <v>3.2759999999999998</v>
       </c>
-      <c r="O48" s="13"/>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O48" s="13">
+        <v>2</v>
+      </c>
+      <c r="P48" s="13"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>42794</v>
       </c>
@@ -3690,9 +3811,12 @@
       <c r="N49" s="5">
         <v>3.66</v>
       </c>
-      <c r="O49" s="13"/>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O49" s="13">
+        <v>2</v>
+      </c>
+      <c r="P49" s="13"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>42794</v>
       </c>
@@ -3735,9 +3859,12 @@
       <c r="N50" s="5">
         <v>3.91</v>
       </c>
-      <c r="O50" s="13"/>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O50" s="13">
+        <v>2</v>
+      </c>
+      <c r="P50" s="13"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>42807</v>
       </c>
@@ -3780,9 +3907,12 @@
       <c r="N51" s="5">
         <v>1.8360000000000001</v>
       </c>
-      <c r="O51" s="13"/>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O51" s="13">
+        <v>2</v>
+      </c>
+      <c r="P51" s="13"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>42955</v>
       </c>
@@ -3825,9 +3955,12 @@
       <c r="N52" s="5">
         <v>2.0870000000000002</v>
       </c>
-      <c r="O52" s="13"/>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O52" s="13">
+        <v>2</v>
+      </c>
+      <c r="P52" s="13"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>42955</v>
       </c>
@@ -3870,9 +4003,12 @@
       <c r="N53" s="5">
         <v>3.484</v>
       </c>
-      <c r="O53" s="13"/>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O53" s="13">
+        <v>2</v>
+      </c>
+      <c r="P53" s="13"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>42976</v>
       </c>
@@ -3915,9 +4051,12 @@
       <c r="N54" s="5">
         <v>3.8780000000000001</v>
       </c>
-      <c r="O54" s="13"/>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O54" s="13">
+        <v>2</v>
+      </c>
+      <c r="P54" s="13"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>43041</v>
       </c>
@@ -3960,9 +4099,12 @@
       <c r="N55" s="5">
         <v>2.278</v>
       </c>
-      <c r="O55" s="13"/>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O55" s="13">
+        <v>2</v>
+      </c>
+      <c r="P55" s="13"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>43040</v>
       </c>
@@ -4005,9 +4147,12 @@
       <c r="N56" s="5">
         <v>3.3879999999999999</v>
       </c>
-      <c r="O56" s="13"/>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O56" s="13">
+        <v>2</v>
+      </c>
+      <c r="P56" s="13"/>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>43048</v>
       </c>
@@ -4050,9 +4195,12 @@
       <c r="N57" s="5">
         <v>1.907</v>
       </c>
-      <c r="O57" s="13"/>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O57" s="13">
+        <v>2</v>
+      </c>
+      <c r="P57" s="13"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>42243</v>
       </c>
@@ -4095,9 +4243,12 @@
       <c r="N58" s="5">
         <v>3.605</v>
       </c>
-      <c r="O58" s="13"/>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O58" s="13">
+        <v>2</v>
+      </c>
+      <c r="P58" s="13"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>42838</v>
       </c>
@@ -4140,11 +4291,11 @@
       <c r="N59" s="3">
         <v>1.2949999999999999</v>
       </c>
-      <c r="O59" s="14" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O59" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>42838</v>
       </c>
@@ -4187,9 +4338,11 @@
       <c r="N60" s="3">
         <v>2.2669999999999999</v>
       </c>
-      <c r="O60" s="14"/>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O60" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>42843</v>
       </c>
@@ -4232,9 +4385,11 @@
       <c r="N61" s="3">
         <v>1.899</v>
       </c>
-      <c r="O61" s="14"/>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O61" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>42907</v>
       </c>
@@ -4277,9 +4432,11 @@
       <c r="N62" s="3">
         <v>3.702</v>
       </c>
-      <c r="O62" s="14"/>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O62" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>42514</v>
       </c>
@@ -4322,9 +4479,11 @@
       <c r="N63" s="3">
         <v>2.012</v>
       </c>
-      <c r="O63" s="14"/>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O63" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>42215</v>
       </c>
@@ -4367,7 +4526,9 @@
       <c r="N64" s="3">
         <v>1.7669999999999999</v>
       </c>
-      <c r="O64" s="14"/>
+      <c r="O64" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
@@ -4412,7 +4573,9 @@
       <c r="N65" s="3">
         <v>3.6179999999999999</v>
       </c>
-      <c r="O65" s="14"/>
+      <c r="O65" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
@@ -4457,7 +4620,9 @@
       <c r="N66" s="3">
         <v>1.593</v>
       </c>
-      <c r="O66" s="14"/>
+      <c r="O66" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
@@ -4502,7 +4667,9 @@
       <c r="N67" s="3">
         <v>2.6150000000000002</v>
       </c>
-      <c r="O67" s="14"/>
+      <c r="O67" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
@@ -4547,7 +4714,9 @@
       <c r="N68" s="3">
         <v>2.2200000000000002</v>
       </c>
-      <c r="O68" s="14"/>
+      <c r="O68" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
@@ -4592,7 +4761,9 @@
       <c r="N69" s="3">
         <v>3.633</v>
       </c>
-      <c r="O69" s="14"/>
+      <c r="O69" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
@@ -4637,7 +4808,9 @@
       <c r="N70" s="3">
         <v>2.1539999999999999</v>
       </c>
-      <c r="O70" s="14"/>
+      <c r="O70" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
@@ -4682,7 +4855,9 @@
       <c r="N71" s="3">
         <v>3.6789999999999998</v>
       </c>
-      <c r="O71" s="14"/>
+      <c r="O71" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
@@ -4727,7 +4902,9 @@
       <c r="N72" s="3">
         <v>3.5910000000000002</v>
       </c>
-      <c r="O72" s="14"/>
+      <c r="O72" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
@@ -4772,7 +4949,9 @@
       <c r="N73" s="3">
         <v>3.59</v>
       </c>
-      <c r="O73" s="14"/>
+      <c r="O73" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
@@ -4817,7 +4996,9 @@
       <c r="N74" s="3">
         <v>2.2040000000000002</v>
       </c>
-      <c r="O74" s="14"/>
+      <c r="O74" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
@@ -4862,7 +5043,9 @@
       <c r="N75" s="3">
         <v>2.3439999999999999</v>
       </c>
-      <c r="O75" s="14"/>
+      <c r="O75" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
@@ -4907,7 +5090,9 @@
       <c r="N76" s="3">
         <v>1.355</v>
       </c>
-      <c r="O76" s="14"/>
+      <c r="O76" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
@@ -4952,7 +5137,9 @@
       <c r="N77" s="3">
         <v>3.3359999999999999</v>
       </c>
-      <c r="O77" s="14"/>
+      <c r="O77" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
@@ -4997,7 +5184,9 @@
       <c r="N78" s="3">
         <v>3.3849999999999998</v>
       </c>
-      <c r="O78" s="14"/>
+      <c r="O78" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
@@ -5042,7 +5231,9 @@
       <c r="N79" s="3">
         <v>2.903</v>
       </c>
-      <c r="O79" s="14"/>
+      <c r="O79" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
@@ -5087,7 +5278,9 @@
       <c r="N80" s="3">
         <v>3.3719999999999999</v>
       </c>
-      <c r="O80" s="14"/>
+      <c r="O80" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
@@ -5132,7 +5325,9 @@
       <c r="N81" s="3">
         <v>3.056</v>
       </c>
-      <c r="O81" s="14"/>
+      <c r="O81" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
@@ -5177,7 +5372,9 @@
       <c r="N82" s="3">
         <v>3.202</v>
       </c>
-      <c r="O82" s="14"/>
+      <c r="O82" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
@@ -5222,7 +5419,9 @@
       <c r="N83" s="3">
         <v>3.1819999999999999</v>
       </c>
-      <c r="O83" s="14"/>
+      <c r="O83" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
@@ -5267,7 +5466,9 @@
       <c r="N84" s="3">
         <v>3.044</v>
       </c>
-      <c r="O84" s="14"/>
+      <c r="O84" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
@@ -5312,7 +5513,9 @@
       <c r="N85" s="3">
         <v>3.1709999999999998</v>
       </c>
-      <c r="O85" s="14"/>
+      <c r="O85" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
@@ -5357,7 +5560,9 @@
       <c r="N86" s="3">
         <v>2.2400000000000002</v>
       </c>
-      <c r="O86" s="14"/>
+      <c r="O86" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
@@ -5402,8 +5607,8 @@
       <c r="N87" s="5">
         <v>3.2829999999999999</v>
       </c>
-      <c r="O87" s="13" t="s">
-        <v>163</v>
+      <c r="O87" s="15">
+        <v>4</v>
       </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
@@ -5449,7 +5654,9 @@
       <c r="N88" s="5">
         <v>2.8809999999999998</v>
       </c>
-      <c r="O88" s="13"/>
+      <c r="O88" s="16">
+        <v>4</v>
+      </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
@@ -5494,7 +5701,9 @@
       <c r="N89" s="5">
         <v>3.13</v>
       </c>
-      <c r="O89" s="13"/>
+      <c r="O89" s="16">
+        <v>4</v>
+      </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
@@ -5539,7 +5748,9 @@
       <c r="N90" s="5">
         <v>3.577</v>
       </c>
-      <c r="O90" s="13"/>
+      <c r="O90" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
@@ -5584,7 +5795,9 @@
       <c r="N91" s="5">
         <v>1.516</v>
       </c>
-      <c r="O91" s="13"/>
+      <c r="O91" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
@@ -5629,7 +5842,9 @@
       <c r="N92" s="5">
         <v>2.742</v>
       </c>
-      <c r="O92" s="13"/>
+      <c r="O92" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
@@ -5674,7 +5889,9 @@
       <c r="N93" s="5">
         <v>2.129</v>
       </c>
-      <c r="O93" s="13"/>
+      <c r="O93" s="16">
+        <v>4</v>
+      </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
@@ -5719,7 +5936,9 @@
       <c r="N94" s="5">
         <v>3.4590000000000001</v>
       </c>
-      <c r="O94" s="13"/>
+      <c r="O94" s="16">
+        <v>4</v>
+      </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
@@ -5764,7 +5983,9 @@
       <c r="N95" s="5">
         <v>3.4609999999999999</v>
       </c>
-      <c r="O95" s="13"/>
+      <c r="O95" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
@@ -5809,7 +6030,9 @@
       <c r="N96" s="5">
         <v>3.0089999999999999</v>
       </c>
-      <c r="O96" s="13"/>
+      <c r="O96" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
@@ -5854,7 +6077,9 @@
       <c r="N97" s="5">
         <v>3.532</v>
       </c>
-      <c r="O97" s="13"/>
+      <c r="O97" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
@@ -5899,7 +6124,9 @@
       <c r="N98" s="5">
         <v>3.18</v>
       </c>
-      <c r="O98" s="13"/>
+      <c r="O98" s="16">
+        <v>4</v>
+      </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
@@ -5944,7 +6171,9 @@
       <c r="N99" s="5">
         <v>3.246</v>
       </c>
-      <c r="O99" s="13"/>
+      <c r="O99" s="16">
+        <v>4</v>
+      </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
@@ -5989,7 +6218,9 @@
       <c r="N100" s="5">
         <v>0.99399999999999999</v>
       </c>
-      <c r="O100" s="13"/>
+      <c r="O100" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
@@ -6034,7 +6265,9 @@
       <c r="N101" s="5">
         <v>1.262</v>
       </c>
-      <c r="O101" s="13"/>
+      <c r="O101" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
@@ -6079,7 +6312,9 @@
       <c r="N102" s="5">
         <v>3.7639999999999998</v>
       </c>
-      <c r="O102" s="13"/>
+      <c r="O102" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
@@ -6124,7 +6359,9 @@
       <c r="N103" s="5">
         <v>2.9430000000000001</v>
       </c>
-      <c r="O103" s="13"/>
+      <c r="O103" s="16">
+        <v>4</v>
+      </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
@@ -6169,7 +6406,9 @@
       <c r="N104" s="5">
         <v>3.2069999999999999</v>
       </c>
-      <c r="O104" s="13"/>
+      <c r="O104" s="16">
+        <v>4</v>
+      </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
@@ -6214,7 +6453,9 @@
       <c r="N105" s="5">
         <v>2.8439999999999999</v>
       </c>
-      <c r="O105" s="13"/>
+      <c r="O105" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
@@ -6259,7 +6500,9 @@
       <c r="N106" s="5">
         <v>2.9449999999999998</v>
       </c>
-      <c r="O106" s="13"/>
+      <c r="O106" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
@@ -6304,7 +6547,9 @@
       <c r="N107" s="5">
         <v>2.028</v>
       </c>
-      <c r="O107" s="13"/>
+      <c r="O107" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
@@ -6349,7 +6594,9 @@
       <c r="N108" s="5">
         <v>3.302</v>
       </c>
-      <c r="O108" s="13"/>
+      <c r="O108" s="16">
+        <v>4</v>
+      </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
@@ -6394,7 +6641,9 @@
       <c r="N109" s="5">
         <v>2.59</v>
       </c>
-      <c r="O109" s="13"/>
+      <c r="O109" s="16">
+        <v>4</v>
+      </c>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
@@ -6439,7 +6688,9 @@
       <c r="N110" s="5">
         <v>1.9239999999999999</v>
       </c>
-      <c r="O110" s="13"/>
+      <c r="O110" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
@@ -6484,7 +6735,9 @@
       <c r="N111" s="5">
         <v>2.1890000000000001</v>
       </c>
-      <c r="O111" s="13"/>
+      <c r="O111" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
@@ -6529,7 +6782,9 @@
       <c r="N112" s="5">
         <v>1.8939999999999999</v>
       </c>
-      <c r="O112" s="13"/>
+      <c r="O112" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
@@ -6574,7 +6829,9 @@
       <c r="N113" s="5">
         <v>2.9980000000000002</v>
       </c>
-      <c r="O113" s="13"/>
+      <c r="O113" s="16">
+        <v>4</v>
+      </c>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
@@ -6619,9 +6876,11 @@
       <c r="N114" s="5">
         <v>2.0630000000000002</v>
       </c>
-      <c r="O114" s="13"/>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O114" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="6">
         <v>44377</v>
       </c>
@@ -6664,8 +6923,8 @@
       <c r="N115" s="8">
         <v>1.3</v>
       </c>
-      <c r="O115" s="9" t="s">
-        <v>164</v>
+      <c r="O115" s="17">
+        <v>5</v>
       </c>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.25">
@@ -6711,7 +6970,9 @@
       <c r="N116" s="8">
         <v>2.194</v>
       </c>
-      <c r="O116" s="9"/>
+      <c r="O116" s="17">
+        <v>5</v>
+      </c>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" s="6">
@@ -6756,7 +7017,9 @@
       <c r="N117" s="8">
         <v>2.9430000000000001</v>
       </c>
-      <c r="O117" s="9"/>
+      <c r="O117" s="17">
+        <v>5</v>
+      </c>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" s="6">
@@ -6801,7 +7064,9 @@
       <c r="N118" s="8">
         <v>1.071</v>
       </c>
-      <c r="O118" s="9"/>
+      <c r="O118" s="17">
+        <v>5</v>
+      </c>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" s="6">
@@ -6846,7 +7111,9 @@
       <c r="N119" s="8">
         <v>0.84299999999999997</v>
       </c>
-      <c r="O119" s="9"/>
+      <c r="O119" s="17">
+        <v>5</v>
+      </c>
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" s="6">
@@ -6891,21 +7158,17 @@
       <c r="N120" s="8">
         <v>2.7010000000000001</v>
       </c>
-      <c r="O120" s="9"/>
+      <c r="O120" s="17">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A3:K122">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:K122">
     <sortCondition ref="J3:J122"/>
     <sortCondition ref="K3:K122"/>
   </sortState>
-  <mergeCells count="7">
-    <mergeCell ref="O115:O120"/>
-    <mergeCell ref="O1:O2"/>
+  <mergeCells count="1">
     <mergeCell ref="L1:N1"/>
-    <mergeCell ref="O3:O30"/>
-    <mergeCell ref="O31:O58"/>
-    <mergeCell ref="O59:O86"/>
-    <mergeCell ref="O87:O114"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6913,6 +7176,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2C6069D784E1B4BB829E8DE81236814" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e00ac7a92cce676ababc74140b7f6d20">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1c6defc0-d543-4e05-a176-12cad6535644" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="24cc1514ac707c54565f0aaf5e71ba5b" ns3:_="">
     <xsd:import namespace="1c6defc0-d543-4e05-a176-12cad6535644"/>
@@ -7044,12 +7313,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -7060,6 +7323,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68293747-BA1D-490E-B1BF-E37D3E9699A8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1c6defc0-d543-4e05-a176-12cad6535644"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{401BE0D9-C0B6-4D76-86D8-CD1DC5699C14}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7077,22 +7356,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68293747-BA1D-490E-B1BF-E37D3E9699A8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1c6defc0-d543-4e05-a176-12cad6535644"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D736EF3E-B982-4480-86EB-3062CC71F940}">
   <ds:schemaRefs>

</xml_diff>